<commit_message>
Contacts - 16 Dec 2024
</commit_message>
<xml_diff>
--- a/TestData/T1137_T1138_Contacts_AffiliatedCompany_NewAffiliation_SaveCancelEditUpdate.xlsx
+++ b/TestData/T1137_T1138_Contacts_AffiliatedCompany_NewAffiliation_SaveCancelEditUpdate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A35D36B-972E-4130-B38B-5DF1A2306D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6309617C-A848-4D24-AA32-16B15D73A296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
     <t>Updated affiliation note.</t>
   </si>
   <si>
-    <t>Ayati Arvind</t>
+    <t>Amanda Donovan</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,7 +680,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:E2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>